<commit_message>
changes to figure notebooks
</commit_message>
<xml_diff>
--- a/Notebooks/data_processed.xlsx
+++ b/Notebooks/data_processed.xlsx
@@ -145,7 +145,7 @@
     <t xml:space="preserve">l_gomp_um</t>
   </si>
   <si>
-    <t xml:space="preserve">gomp_growth_stops_10</t>
+    <t xml:space="preserve">ts_10</t>
   </si>
   <si>
     <t xml:space="preserve">tm_um</t>
@@ -15771,23 +15771,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -15798,11 +15781,11 @@
   </sheetPr>
   <dimension ref="A1:AT161"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP2" activeCellId="0" sqref="AP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="16.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="16.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>

</xml_diff>